<commit_message>
updated folder and subfolder of some CI's
</commit_message>
<xml_diff>
--- a/Lhub_CIList.xlsx
+++ b/Lhub_CIList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\Project management\Learning-hub project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Farah\Desktop\V1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="58">
   <si>
     <t>CI ID</t>
   </si>
@@ -167,13 +167,37 @@
     <t>Lhub_CI_21</t>
   </si>
   <si>
-    <t>hight level design document</t>
-  </si>
-  <si>
     <t>wire frame</t>
   </si>
   <si>
     <t>design PR sheet</t>
+  </si>
+  <si>
+    <t>Diagrams</t>
+  </si>
+  <si>
+    <t>Diagrams/ERD</t>
+  </si>
+  <si>
+    <t>Diagrams/UseCase</t>
+  </si>
+  <si>
+    <t>Diagrams/classDiagram</t>
+  </si>
+  <si>
+    <t>Diagrams/High Level design</t>
+  </si>
+  <si>
+    <t>Diagrams/Data Flow design</t>
+  </si>
+  <si>
+    <t>Diagrams/sequence Diagram</t>
+  </si>
+  <si>
+    <t>software design document</t>
+  </si>
+  <si>
+    <t>Diagrams/WireFrames</t>
   </si>
 </sst>
 </file>
@@ -544,9 +568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EU22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -554,7 +576,7 @@
     <col min="2" max="2" width="47.140625" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="37.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:151" s="1" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.35">
@@ -838,7 +860,7 @@
         <v>27</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -854,7 +876,7 @@
         <v>28</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -880,7 +902,7 @@
         <v>31</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -895,8 +917,14 @@
       <c r="C14" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:151" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="D14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:151" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>33</v>
       </c>
@@ -905,6 +933,12 @@
       </c>
       <c r="C15" s="4" t="s">
         <v>19</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:151" ht="19.5" x14ac:dyDescent="0.25">
@@ -917,8 +951,14 @@
       <c r="C16" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="D16" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>35</v>
       </c>
@@ -928,8 +968,14 @@
       <c r="C17" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="D17" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>40</v>
       </c>
@@ -939,8 +985,14 @@
       <c r="C18" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="D18" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>41</v>
       </c>
@@ -950,39 +1002,55 @@
       <c r="C19" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="D21" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>46</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
     </row>
   </sheetData>
   <dataValidations count="2">

</xml_diff>